<commit_message>
Add support for percent of total, percent of col, and percent of col for the show data as pivot field setting.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
   <si>
     <t>Transaction</t>
   </si>
@@ -91,6 +91,27 @@
   </si>
   <si>
     <t>Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Total Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>Total Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>January Total</t>
+  </si>
+  <si>
+    <t>February Total</t>
+  </si>
+  <si>
+    <t>March Total</t>
   </si>
 </sst>
 </file>
@@ -166,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,6 +201,10 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -316,7 +341,101 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B18:K22" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="2" baseItem="1" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -401,13 +520,244 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0" numFmtId="10">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
-          <x14:dataField pivotShowAs="percentOfParentRow"/>
-        </ext>
-      </extLst>
-    </dataField>
+    <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="-2"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="20">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -881,17 +1231,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -912,8 +1282,8 @@
       <c r="C3" s="6">
         <v>0.22192458169477189</v>
       </c>
-      <c r="D3" s="6">
-        <v>0.2</v>
+      <c r="D3" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -923,8 +1293,8 @@
       <c r="C4" s="6">
         <v>0.20934143676453557</v>
       </c>
-      <c r="D4" s="6">
-        <v>0.66666666666666663</v>
+      <c r="D4" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -934,8 +1304,8 @@
       <c r="C5" s="6">
         <v>1.2583144930236304E-2</v>
       </c>
-      <c r="D5" s="6">
-        <v>0.33333333333333331</v>
+      <c r="D5" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -945,8 +1315,8 @@
       <c r="C6" s="6">
         <v>0.51888478793951631</v>
       </c>
-      <c r="D6" s="6">
-        <v>0.66666666666666663</v>
+      <c r="D6" s="7">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -956,8 +1326,8 @@
       <c r="C7" s="6">
         <v>0.20934143676453557</v>
       </c>
-      <c r="D7" s="6">
-        <v>0.2</v>
+      <c r="D7" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -967,8 +1337,8 @@
       <c r="C8" s="6">
         <v>0.10020191441044517</v>
       </c>
-      <c r="D8" s="6">
-        <v>0.6</v>
+      <c r="D8" s="7">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -978,8 +1348,8 @@
       <c r="C9" s="6">
         <v>0.20934143676453557</v>
       </c>
-      <c r="D9" s="6">
-        <v>0.2</v>
+      <c r="D9" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -989,8 +1359,8 @@
       <c r="C10" s="6">
         <v>0.25919063036571183</v>
       </c>
-      <c r="D10" s="6">
-        <v>0.13333333333333333</v>
+      <c r="D10" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -1000,8 +1370,8 @@
       <c r="C11" s="6">
         <v>0.20934143676453557</v>
       </c>
-      <c r="D11" s="6">
-        <v>0.5</v>
+      <c r="D11" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -1011,8 +1381,8 @@
       <c r="C12" s="6">
         <v>4.9849193601176241E-2</v>
       </c>
-      <c r="D12" s="6">
-        <v>0.5</v>
+      <c r="D12" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -1022,8 +1392,641 @@
       <c r="C13" s="6">
         <v>1</v>
       </c>
-      <c r="D13" s="6">
-        <v>1</v>
+      <c r="D13" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.62802431029360672</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.62802431029360672</v>
+      </c>
+      <c r="E21" s="6">
+        <v>4.9849193601176241E-2</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.10020191441044517</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.15005110801162141</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.20934143676453557</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1.2583144930236304E-2</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.22192458169477189</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7">
+        <v>5</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>6</v>
+      </c>
+      <c r="G22" s="7">
+        <v>7</v>
+      </c>
+      <c r="H22" s="7">
+        <v>2</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>3</v>
+      </c>
+      <c r="K22" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.94329990470572223</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.40344492964580303</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.80767362797474507</v>
+      </c>
+      <c r="F34" s="7">
+        <v>2</v>
+      </c>
+      <c r="G34" s="7">
+        <v>2</v>
+      </c>
+      <c r="H34" s="7">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0.62802431029360672</v>
+      </c>
+      <c r="J34" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.19232637202525499</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
+      <c r="I36" s="6">
+        <v>4.9849193601176241E-2</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.193110140708394</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7">
+        <v>6</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="6">
+        <v>0.10020191441044517</v>
+      </c>
+      <c r="J37" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="7"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.40344492964580303</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7">
+        <v>2</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="6">
+        <v>0.20934143676453557</v>
+      </c>
+      <c r="J39" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="6">
+        <v>5.6700095294277802E-2</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="6">
+        <v>1.2583144930236304E-2</v>
+      </c>
+      <c r="J40" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>3</v>
+      </c>
+      <c r="G41" s="7">
+        <v>10</v>
+      </c>
+      <c r="H41" s="7">
+        <v>2</v>
+      </c>
+      <c r="I41" s="6">
+        <v>1</v>
+      </c>
+      <c r="J41" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D50" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E50" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="6">
+        <v>0</v>
+      </c>
+      <c r="D52" s="6">
+        <v>0</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="6">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="6">
+        <v>0</v>
+      </c>
+      <c r="D53" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E53" s="6">
+        <v>0</v>
+      </c>
+      <c r="F53" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0</v>
+      </c>
+      <c r="D55" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6">
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D56" s="6">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+      <c r="F56" s="6">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="7">
+        <v>415.75</v>
+      </c>
+      <c r="D59" s="7">
+        <v>415.75</v>
+      </c>
+      <c r="E59" s="7">
+        <v>415.75</v>
+      </c>
+      <c r="F59" s="7">
+        <v>1247.25</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7">
+        <v>99</v>
+      </c>
+      <c r="F61" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7">
+        <v>199</v>
+      </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7">
+        <v>415.75</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="7">
+        <v>24.99</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="6">
+        <v>1</v>
+      </c>
+      <c r="D66" s="6">
+        <v>1</v>
+      </c>
+      <c r="E66" s="6">
+        <v>1</v>
+      </c>
+      <c r="F66" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="7">
+        <v>440.74</v>
+      </c>
+      <c r="D67" s="7">
+        <v>1030.5</v>
+      </c>
+      <c r="E67" s="7">
+        <v>514.75</v>
+      </c>
+      <c r="F67" s="7">
+        <v>1985.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for "% of" show data as setting option.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="62" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -341,7 +341,247 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="62" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="-2"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="20">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="62" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="62" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B18:K22" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -434,8 +674,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="62" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -521,243 +761,6 @@
   <dataFields count="2">
     <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
     <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="-2"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="20">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="3"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="-2"/>
-    <field x="1"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1233,21 +1236,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" customWidth="1"/>
@@ -1554,14 +1557,30 @@
       <c r="B33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="7"/>
+      <c r="C33" s="6">
+        <v>0.94329990470572223</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.40344492964580303</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.80767362797474507</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7">
+        <v>2</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0.62802431029360672</v>
+      </c>
+      <c r="J33" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
@@ -1596,14 +1615,28 @@
       <c r="B35" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.193110140708394</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.19232637202525499</v>
+      </c>
       <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="7"/>
+      <c r="G35" s="7">
+        <v>6</v>
+      </c>
+      <c r="H35" s="7">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6">
+        <v>0.15005110801162141</v>
+      </c>
+      <c r="J35" s="7">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
@@ -1659,14 +1692,28 @@
       <c r="B38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="C38" s="6">
+        <v>5.6700095294277802E-2</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.40344492964580303</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
+      <c r="G38" s="7">
+        <v>2</v>
+      </c>
       <c r="H38" s="7"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="7"/>
+      <c r="I38" s="6">
+        <v>0.22192458169477189</v>
+      </c>
+      <c r="J38" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">

</xml_diff>

<commit_message>
Add support for show data as percent of parent.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="62" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
   <si>
     <t>Transaction</t>
   </si>
@@ -341,7 +341,229 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="62" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B76:K88" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="-2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="2" baseItem="1" numFmtId="10">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
+          <x14:dataField pivotShowAs="percentOfParent"/>
+        </ext>
+      </extLst>
+    </dataField>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -468,8 +690,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="62" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -580,8 +802,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="62" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B18:K22" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -664,103 +886,6 @@
   <dataFields count="2">
     <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="2" baseItem="1" numFmtId="10"/>
     <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="62" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1234,33 +1359,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K67"/>
+  <dimension ref="B2:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" customWidth="1"/>
     <col min="21" max="21" width="9.28515625" customWidth="1"/>
     <col min="22" max="22" width="11.42578125" customWidth="1"/>
     <col min="23" max="23" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -2029,7 +2152,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="s">
         <v>14</v>
       </c>
@@ -2042,7 +2165,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>24</v>
       </c>
@@ -2059,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
         <v>23</v>
       </c>
@@ -2074,6 +2197,298 @@
       </c>
       <c r="F67" s="7">
         <v>1985.99</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C76" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>25</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" t="s">
+        <v>26</v>
+      </c>
+      <c r="H77" t="s">
+        <v>13</v>
+      </c>
+      <c r="J77" t="s">
+        <v>27</v>
+      </c>
+      <c r="K77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" t="s">
+        <v>9</v>
+      </c>
+      <c r="I78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="6">
+        <v>1</v>
+      </c>
+      <c r="D80" s="6">
+        <v>1</v>
+      </c>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6">
+        <v>0</v>
+      </c>
+      <c r="I80" s="6">
+        <v>1</v>
+      </c>
+      <c r="J80" s="6">
+        <v>1</v>
+      </c>
+      <c r="K80" s="6"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="6">
+        <v>1</v>
+      </c>
+      <c r="D81" s="6">
+        <v>1</v>
+      </c>
+      <c r="E81" s="6">
+        <v>0</v>
+      </c>
+      <c r="F81" s="6">
+        <v>1</v>
+      </c>
+      <c r="G81" s="6">
+        <v>1</v>
+      </c>
+      <c r="H81" s="6">
+        <v>1</v>
+      </c>
+      <c r="I81" s="6">
+        <v>0</v>
+      </c>
+      <c r="J81" s="6">
+        <v>1</v>
+      </c>
+      <c r="K81" s="6"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="6">
+        <v>1</v>
+      </c>
+      <c r="D82" s="6">
+        <v>1</v>
+      </c>
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+      <c r="F82" s="6">
+        <v>0</v>
+      </c>
+      <c r="G82" s="6">
+        <v>1</v>
+      </c>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="7">
+        <v>2</v>
+      </c>
+      <c r="D84" s="7">
+        <v>2</v>
+      </c>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7">
+        <v>1</v>
+      </c>
+      <c r="J84" s="7">
+        <v>1</v>
+      </c>
+      <c r="K84" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2</v>
+      </c>
+      <c r="D85" s="7">
+        <v>2</v>
+      </c>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7">
+        <v>6</v>
+      </c>
+      <c r="G85" s="7">
+        <v>6</v>
+      </c>
+      <c r="H85" s="7">
+        <v>2</v>
+      </c>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7">
+        <v>2</v>
+      </c>
+      <c r="K85" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="7">
+        <v>1</v>
+      </c>
+      <c r="D86" s="7">
+        <v>1</v>
+      </c>
+      <c r="E86" s="7">
+        <v>1</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7">
+        <v>1</v>
+      </c>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="6">
+        <v>1</v>
+      </c>
+      <c r="D87" s="6">
+        <v>1</v>
+      </c>
+      <c r="E87" s="6">
+        <v>0.33221476510067116</v>
+      </c>
+      <c r="F87" s="6">
+        <v>0.66778523489932884</v>
+      </c>
+      <c r="G87" s="6">
+        <v>1</v>
+      </c>
+      <c r="H87" s="6">
+        <v>0.94329990470572223</v>
+      </c>
+      <c r="I87" s="6">
+        <v>5.6700095294277802E-2</v>
+      </c>
+      <c r="J87" s="6">
+        <v>1</v>
+      </c>
+      <c r="K87" s="6"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="7">
+        <v>5</v>
+      </c>
+      <c r="D88" s="7">
+        <v>5</v>
+      </c>
+      <c r="E88" s="7">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7">
+        <v>6</v>
+      </c>
+      <c r="G88" s="7">
+        <v>7</v>
+      </c>
+      <c r="H88" s="7">
+        <v>2</v>
+      </c>
+      <c r="I88" s="7">
+        <v>1</v>
+      </c>
+      <c r="J88" s="7">
+        <v>3</v>
+      </c>
+      <c r="K88" s="7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix null cast issue causing an exception while refreshing pivot tables.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="29">
   <si>
     <t>Transaction</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>March Total</t>
+  </si>
+  <si>
+    <t>Count of Wholesale Price</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,489 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B93:C97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Wholesale Price" fld="4" subtotal="count" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="2" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="-2"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="20">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B18:K22" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="2" baseItem="1" numFmtId="10"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="2" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B76:K88" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -454,437 +939,6 @@
         </ext>
       </extLst>
     </dataField>
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="1" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="1" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="-2"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="20">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="3"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="-2"/>
-    <field x="1"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B18:K22" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </colFields>
-  <colItems count="9">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Wholesale Price" fld="4" showDataAs="percentOfTotal" baseField="2" baseItem="1" numFmtId="10"/>
     <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1359,16 +1413,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K88"/>
+  <dimension ref="B2:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
@@ -2491,6 +2545,46 @@
         <v>15</v>
       </c>
     </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="6">
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="6">
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="6">
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bugs/13335 percent column total (#298)
* staging

* added tests

* added comments, small refactor

* remove helper method
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableShowDataAs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A41BE-A1D4-438D-BD7B-1A0821633E00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24375" windowHeight="11250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24375" windowHeight="11250" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="78" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="31">
   <si>
     <t>Transaction</t>
   </si>
@@ -116,11 +117,17 @@
   <si>
     <t>Count of Wholesale Price</t>
   </si>
+  <si>
+    <t>Sum of Total</t>
+  </si>
+  <si>
+    <t>Total Sum of Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -227,7 +234,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43503.405086574072" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="7">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43503.405086574072" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="7" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B2:H9" sheet="Sheet1"/>
   </cacheSource>
@@ -276,7 +283,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="7">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="7">
   <r>
     <n v="20100076"/>
     <x v="0"/>
@@ -344,7 +351,140 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18B851D6-861E-44AB-AFDD-9FAE76387D79}" name="PivotTable10" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B110:L123" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0" numFmtId="10">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
+          <x14:dataField pivotShowAs="percentOfParentCol"/>
+        </ext>
+      </extLst>
+    </dataField>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000005000000}" name="PivotTable7" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B93:C97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -390,12 +530,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -487,140 +630,119 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="2" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CC88BD8B-A744-4BAC-9D52-8C5FD9C9D913}" name="PivotTable8" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B100:L106" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
         <item x="0"/>
         <item x="2"/>
         <item x="1"/>
         <item x="3"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
     <field x="-2"/>
-    <field x="2"/>
     <field x="3"/>
-  </rowFields>
-  <rowItems count="20">
+  </colFields>
+  <colItems count="10">
     <i>
       <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
       <x v="2"/>
     </i>
-    <i r="2">
+    <i r="1">
       <x v="3"/>
     </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i i="1">
       <x v="1"/>
+      <x/>
     </i>
     <i r="1" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="3"/>
+      <x v="1"/>
     </i>
     <i r="1" i="1">
       <x v="2"/>
     </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
+    <i r="1" i="1">
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
     </i>
     <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0" numFmtId="10">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
+          <x14:dataField pivotShowAs="percentOfParentCol"/>
+        </ext>
+      </extLst>
+    </dataField>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000002000000}" name="PivotTable3" cacheId="78" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B30:J41" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -727,12 +849,146 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000003000000}" name="PivotTable4" cacheId="78" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B46:F67" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="-2"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="20">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" showDataAs="percentOfCol" baseField="2" baseItem="0" numFmtId="10"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable2" cacheId="78" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B18:K22" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -821,12 +1077,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="2" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000004000000}" name="PivotTable6" cacheId="78" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B76:K88" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -945,6 +1204,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1212,7 +1474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1412,25 +1674,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="13" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
@@ -2577,12 +2841,563 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C97" s="6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C100" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" t="s">
+        <v>20</v>
+      </c>
+      <c r="K101" t="s">
+        <v>30</v>
+      </c>
+      <c r="L101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" t="s">
+        <v>9</v>
+      </c>
+      <c r="H102" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" t="s">
+        <v>11</v>
+      </c>
+      <c r="J102" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" s="6">
+        <v>1</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0</v>
+      </c>
+      <c r="E103" s="6">
+        <v>0</v>
+      </c>
+      <c r="F103" s="6">
+        <v>0</v>
+      </c>
+      <c r="G103" s="7">
+        <v>5</v>
+      </c>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="6">
+        <v>1</v>
+      </c>
+      <c r="L103" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="6">
+        <v>0</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0</v>
+      </c>
+      <c r="E104" s="6">
+        <v>7.6566125290023199E-2</v>
+      </c>
+      <c r="F104" s="6">
+        <v>0.92343387470997684</v>
+      </c>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7">
+        <v>1</v>
+      </c>
+      <c r="J104" s="7">
+        <v>6</v>
+      </c>
+      <c r="K104" s="6">
+        <v>1</v>
+      </c>
+      <c r="L104" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="6">
+        <v>0.97082277668157246</v>
+      </c>
+      <c r="D105" s="6">
+        <v>2.9177223318427533E-2</v>
+      </c>
+      <c r="E105" s="6">
+        <v>0</v>
+      </c>
+      <c r="F105" s="6">
+        <v>0</v>
+      </c>
+      <c r="G105" s="7">
+        <v>2</v>
+      </c>
+      <c r="H105" s="7">
+        <v>1</v>
+      </c>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="6">
+        <v>1</v>
+      </c>
+      <c r="L105" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="6">
+        <v>0.68828874425292796</v>
+      </c>
+      <c r="D106" s="6">
+        <v>5.9102605339337406E-3</v>
+      </c>
+      <c r="E106" s="6">
+        <v>2.3413997313302935E-2</v>
+      </c>
+      <c r="F106" s="6">
+        <v>0.2823869978998354</v>
+      </c>
+      <c r="G106" s="7">
+        <v>7</v>
+      </c>
+      <c r="H106" s="7">
+        <v>1</v>
+      </c>
+      <c r="I106" s="7">
+        <v>1</v>
+      </c>
+      <c r="J106" s="7">
+        <v>6</v>
+      </c>
+      <c r="K106" s="6">
+        <v>1</v>
+      </c>
+      <c r="L106" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C110" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>29</v>
+      </c>
+      <c r="G111" t="s">
+        <v>20</v>
+      </c>
+      <c r="K111" t="s">
+        <v>30</v>
+      </c>
+      <c r="L111" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" t="s">
+        <v>9</v>
+      </c>
+      <c r="H112" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" t="s">
+        <v>11</v>
+      </c>
+      <c r="J112" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="6">
+        <v>1</v>
+      </c>
+      <c r="D113" s="6">
+        <v>0</v>
+      </c>
+      <c r="E113" s="6">
+        <v>0</v>
+      </c>
+      <c r="F113" s="6">
+        <v>0</v>
+      </c>
+      <c r="G113" s="7">
+        <v>5</v>
+      </c>
+      <c r="H113" s="7"/>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="6">
+        <v>1</v>
+      </c>
+      <c r="L113" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" s="6">
+        <v>1</v>
+      </c>
+      <c r="D114" s="6">
+        <v>0</v>
+      </c>
+      <c r="E114" s="6">
+        <v>0</v>
+      </c>
+      <c r="F114" s="6">
+        <v>0</v>
+      </c>
+      <c r="G114" s="7">
+        <v>2</v>
+      </c>
+      <c r="H114" s="7"/>
+      <c r="I114" s="7"/>
+      <c r="J114" s="7"/>
+      <c r="K114" s="6">
+        <v>1</v>
+      </c>
+      <c r="L114" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" s="6">
+        <v>1</v>
+      </c>
+      <c r="D115" s="6">
+        <v>0</v>
+      </c>
+      <c r="E115" s="6">
+        <v>0</v>
+      </c>
+      <c r="F115" s="6">
+        <v>0</v>
+      </c>
+      <c r="G115" s="7">
+        <v>2</v>
+      </c>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="6">
+        <v>1</v>
+      </c>
+      <c r="L115" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" s="6">
+        <v>1</v>
+      </c>
+      <c r="D116" s="6">
+        <v>0</v>
+      </c>
+      <c r="E116" s="6">
+        <v>0</v>
+      </c>
+      <c r="F116" s="6">
+        <v>0</v>
+      </c>
+      <c r="G116" s="7">
+        <v>1</v>
+      </c>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="6">
+        <v>1</v>
+      </c>
+      <c r="L116" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" s="6">
+        <v>0</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0</v>
+      </c>
+      <c r="E117" s="6">
+        <v>7.6566125290023199E-2</v>
+      </c>
+      <c r="F117" s="6">
+        <v>0.92343387470997684</v>
+      </c>
+      <c r="G117" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="I117" s="7">
+        <v>1</v>
+      </c>
+      <c r="J117" s="7">
+        <v>6</v>
+      </c>
+      <c r="K117" s="6">
+        <v>1</v>
+      </c>
+      <c r="L117" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="6">
+        <v>0</v>
+      </c>
+      <c r="D118" s="6">
+        <v>0</v>
+      </c>
+      <c r="E118" s="6">
+        <v>0</v>
+      </c>
+      <c r="F118" s="6">
+        <v>1</v>
+      </c>
+      <c r="G118" s="7"/>
+      <c r="H118" s="7"/>
+      <c r="I118" s="7"/>
+      <c r="J118" s="7">
+        <v>6</v>
+      </c>
+      <c r="K118" s="6">
+        <v>1</v>
+      </c>
+      <c r="L118" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="6">
+        <v>0</v>
+      </c>
+      <c r="D119" s="6">
+        <v>0</v>
+      </c>
+      <c r="E119" s="6">
+        <v>1</v>
+      </c>
+      <c r="F119" s="6">
+        <v>0</v>
+      </c>
+      <c r="G119" s="7"/>
+      <c r="H119" s="7"/>
+      <c r="I119" s="7">
+        <v>1</v>
+      </c>
+      <c r="J119" s="7"/>
+      <c r="K119" s="6">
+        <v>1</v>
+      </c>
+      <c r="L119" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="6">
+        <v>0.97082277668157246</v>
+      </c>
+      <c r="D120" s="6">
+        <v>2.9177223318427533E-2</v>
+      </c>
+      <c r="E120" s="6">
+        <v>0</v>
+      </c>
+      <c r="F120" s="6">
+        <v>0</v>
+      </c>
+      <c r="G120" s="7">
+        <v>2</v>
+      </c>
+      <c r="H120" s="7">
+        <v>1</v>
+      </c>
+      <c r="I120" s="7"/>
+      <c r="J120" s="7"/>
+      <c r="K120" s="6">
+        <v>1</v>
+      </c>
+      <c r="L120" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" s="6">
+        <v>0</v>
+      </c>
+      <c r="D121" s="6">
+        <v>1</v>
+      </c>
+      <c r="E121" s="6">
+        <v>0</v>
+      </c>
+      <c r="F121" s="6">
+        <v>0</v>
+      </c>
+      <c r="G121" s="7"/>
+      <c r="H121" s="7">
+        <v>1</v>
+      </c>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="6">
+        <v>1</v>
+      </c>
+      <c r="L121" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" s="6">
+        <v>1</v>
+      </c>
+      <c r="D122" s="6">
+        <v>0</v>
+      </c>
+      <c r="E122" s="6">
+        <v>0</v>
+      </c>
+      <c r="F122" s="6">
+        <v>0</v>
+      </c>
+      <c r="G122" s="7">
+        <v>2</v>
+      </c>
+      <c r="H122" s="7"/>
+      <c r="I122" s="7"/>
+      <c r="J122" s="7"/>
+      <c r="K122" s="6">
+        <v>1</v>
+      </c>
+      <c r="L122" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C123" s="6">
+        <v>0.68828874425292796</v>
+      </c>
+      <c r="D123" s="6">
+        <v>5.9102605339337406E-3</v>
+      </c>
+      <c r="E123" s="6">
+        <v>2.3413997313302935E-2</v>
+      </c>
+      <c r="F123" s="6">
+        <v>0.2823869978998354</v>
+      </c>
+      <c r="G123" s="7">
+        <v>7</v>
+      </c>
+      <c r="H123" s="7">
+        <v>1</v>
+      </c>
+      <c r="I123" s="7">
+        <v>1</v>
+      </c>
+      <c r="J123" s="7">
+        <v>6</v>
+      </c>
+      <c r="K123" s="6">
+        <v>1</v>
+      </c>
+      <c r="L123" s="7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>